<commit_message>
workign wiht lab hours
</commit_message>
<xml_diff>
--- a/LabSignup/LabSignup/bin/Debug/ExcelFiles/LabDetails.xlsx
+++ b/LabSignup/LabSignup/bin/Debug/ExcelFiles/LabDetails.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CODING\LabSignup\LabSignup\LabSignup\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CODING\LabSignup\LabSignup\LabSignup\bin\Debug\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B30444-A418-4843-9ADA-05BAC833CEEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941C1EF7-09D4-4916-AAC3-A21713C5F868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="2940" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32985" yWindow="3165" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>LabName</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>What are STD's</t>
+  </si>
+  <si>
+    <t>6:45PM</t>
   </si>
 </sst>
 </file>
@@ -382,7 +385,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,7 +421,7 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>